<commit_message>
add introductory presenations and zoom link to schedule
</commit_message>
<xml_diff>
--- a/Schedule-draft.xlsx
+++ b/Schedule-draft.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/tk18583_bristol_ac_uk/Documents/Documents/GIT/QUSS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="8_{68D395C2-8711-4946-9AFB-D66B5FF3FFAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F724D45-BB1A-49B1-BDB6-87D326BDFE23}"/>
+  <xr:revisionPtr revIDLastSave="121" documentId="8_{68D395C2-8711-4946-9AFB-D66B5FF3FFAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF9DC3D2-28F2-44DC-B830-98C6A2E21A6B}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0284D646-AD08-40C3-A716-CD9E6437E99F}"/>
+    <workbookView xWindow="-27660" yWindow="1140" windowWidth="21600" windowHeight="11265" xr2:uid="{0284D646-AD08-40C3-A716-CD9E6437E99F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,14 +56,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="50">
   <si>
     <t>Period</t>
   </si>
   <si>
-    <t xml:space="preserve">Week </t>
-  </si>
-  <si>
     <t>Teaching Block 1</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>Introduction and welcome back</t>
-  </si>
-  <si>
     <t>Total seminars</t>
   </si>
   <si>
@@ -115,18 +109,9 @@
     <t>Yes</t>
   </si>
   <si>
-    <t xml:space="preserve">Mary Abed Al Ahad &lt;maaa1@st-andrews.ac.uk&gt; - </t>
-  </si>
-  <si>
-    <t>Reading seminar</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
-    <t>In person</t>
-  </si>
-  <si>
     <t>Room</t>
   </si>
   <si>
@@ -136,20 +121,98 @@
     <t>SR2</t>
   </si>
   <si>
-    <t>Tom Cantellow and Rui Sun - Progress presentations</t>
-  </si>
-  <si>
     <t>Wills Memorial Building 3.23</t>
   </si>
   <si>
     <t>Yes - 5pm</t>
+  </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>Reading seminar- robustness in Quantitative research</t>
+  </si>
+  <si>
+    <t>Emmanouil Tranos: Using the web to predict regional trade flows: material and immaterial regional interdependencies</t>
+  </si>
+  <si>
+    <t>Levi Wolf: Consistent urban areas for global urban polimetrics</t>
+  </si>
+  <si>
+    <t>Mary Abed Al Ahad</t>
+  </si>
+  <si>
+    <t>Introductory presentations - Tao &amp; Ekaterina</t>
+  </si>
+  <si>
+    <t>Hannah Budnitz</t>
+  </si>
+  <si>
+    <t>TBC</t>
+  </si>
+  <si>
+    <t>Karyn Morrissey: Area level Deprivation and Monthly COVID-19 cases: The impact of Government Policy in England</t>
+  </si>
+  <si>
+    <t>Caitlin Robinson</t>
+  </si>
+  <si>
+    <t>Dianna Smith</t>
+  </si>
+  <si>
+    <t>Tom Cantellow and Rui Sun - Progress presentations TBC</t>
+  </si>
+  <si>
+    <t>Introductory presentation - Mark &amp; progress presentation - Tom Cantellow</t>
+  </si>
+  <si>
+    <t>Blended</t>
+  </si>
+  <si>
+    <t>Link to zoom</t>
+  </si>
+  <si>
+    <t>https://bristol-ac-uk.zoom.us/j/97858763043?pwd=bVp6RmRTN1J0UE00M1NLcGpLWkFFQT09</t>
+  </si>
+  <si>
+    <t>https://bristol-ac-uk.zoom.us/j/97858763043?pwd=bVp6RmRTN1J0UE00M1NLcGpLWkFFQT10</t>
+  </si>
+  <si>
+    <t>https://bristol-ac-uk.zoom.us/j/97858763043?pwd=bVp6RmRTN1J0UE00M1NLcGpLWkFFQT11</t>
+  </si>
+  <si>
+    <t>https://bristol-ac-uk.zoom.us/j/97858763043?pwd=bVp6RmRTN1J0UE00M1NLcGpLWkFFQT12</t>
+  </si>
+  <si>
+    <t>https://bristol-ac-uk.zoom.us/j/97858763043?pwd=bVp6RmRTN1J0UE00M1NLcGpLWkFFQT13</t>
+  </si>
+  <si>
+    <t>https://bristol-ac-uk.zoom.us/j/97858763043?pwd=bVp6RmRTN1J0UE00M1NLcGpLWkFFQT14</t>
+  </si>
+  <si>
+    <t>https://bristol-ac-uk.zoom.us/j/97858763043?pwd=bVp6RmRTN1J0UE00M1NLcGpLWkFFQT15</t>
+  </si>
+  <si>
+    <t>https://bristol-ac-uk.zoom.us/j/97858763043?pwd=bVp6RmRTN1J0UE00M1NLcGpLWkFFQT16</t>
+  </si>
+  <si>
+    <t>https://bristol-ac-uk.zoom.us/j/97858763043?pwd=bVp6RmRTN1J0UE00M1NLcGpLWkFFQT17</t>
+  </si>
+  <si>
+    <t>https://bristol-ac-uk.zoom.us/j/97858763043?pwd=bVp6RmRTN1J0UE00M1NLcGpLWkFFQT18</t>
+  </si>
+  <si>
+    <t>https://bristol-ac-uk.zoom.us/j/97858763043?pwd=bVp6RmRTN1J0UE00M1NLcGpLWkFFQT19</t>
+  </si>
+  <si>
+    <t>https://bristol-ac-uk.zoom.us/j/97858763043?pwd=bVp6RmRTN1J0UE00M1NLcGpLWkFFQT20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,8 +232,28 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF24292F"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF24292F"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,6 +269,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -240,10 +329,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -259,8 +349,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -573,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF015926-2187-4219-ACCD-3CE7CABC6AE9}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -584,36 +688,42 @@
     <col min="2" max="2" width="11.7265625" customWidth="1"/>
     <col min="3" max="3" width="24.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" style="3"/>
+    <col min="6" max="6" width="15.08984375" customWidth="1"/>
+    <col min="7" max="7" width="11.90625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="18.81640625" customWidth="1"/>
+    <col min="9" max="9" width="68" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -621,18 +731,19 @@
         <v>44462</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E2" s="7"/>
-      <c r="G2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F2" s="7"/>
+      <c r="H2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -640,25 +751,28 @@
         <v>44469</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -666,21 +780,26 @@
         <v>44476</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -688,21 +807,26 @@
         <v>44483</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -710,21 +834,24 @@
         <v>44490</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -732,21 +859,26 @@
         <v>44497</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -754,23 +886,26 @@
         <v>44504</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -778,21 +913,26 @@
         <v>44511</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -800,21 +940,26 @@
         <v>44518</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -822,21 +967,26 @@
         <v>44525</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -844,21 +994,26 @@
         <v>44532</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -866,23 +1021,26 @@
         <v>44539</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -890,19 +1048,22 @@
         <v>44546</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -910,18 +1071,19 @@
         <v>44553</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E15" s="7"/>
-      <c r="G15" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F15" s="7"/>
+      <c r="H15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -929,445 +1091,897 @@
         <v>44560</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E16" s="7"/>
-      <c r="G16" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F16" s="7"/>
+      <c r="H16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
         <v>15</v>
       </c>
       <c r="B17" s="4">
-        <v>44567</v>
+        <v>44202</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="H17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="3">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4">
+        <v>44209</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="7"/>
-      <c r="G17" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="3">
-        <v>16</v>
-      </c>
-      <c r="B18" s="4">
-        <v>44574</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="D18" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E18" s="7"/>
-      <c r="G18" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F18" s="7"/>
+      <c r="H18" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>17</v>
       </c>
       <c r="B19" s="4">
-        <v>44581</v>
+        <v>44216</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E19" s="8"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F19" s="8"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>18</v>
       </c>
       <c r="B20" s="4">
-        <v>44588</v>
+        <v>44223</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E20" s="8"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F20" s="8"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>19</v>
       </c>
       <c r="B21" s="4">
-        <v>44595</v>
+        <v>44230</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E21" s="8"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F21" s="8"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>20</v>
       </c>
       <c r="B22" s="4">
-        <v>44602</v>
+        <v>44237</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E22" s="8"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F22" s="8"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="5"/>
+    </row>
+    <row r="23" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>21</v>
       </c>
       <c r="B23" s="4">
-        <v>44609</v>
+        <v>44244</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E23" s="8"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F23" s="8"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>22</v>
       </c>
       <c r="B24" s="4">
-        <v>44616</v>
+        <v>44251</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E24" s="8"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="5"/>
-    </row>
-    <row r="25" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F24" s="8"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="5"/>
+    </row>
+    <row r="25" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>23</v>
       </c>
       <c r="B25" s="4">
-        <v>44623</v>
+        <v>44258</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E25" s="8"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="5"/>
-    </row>
-    <row r="26" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F25" s="8"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>24</v>
       </c>
       <c r="B26" s="4">
-        <v>44630</v>
+        <v>44265</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E26" s="8"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="5"/>
-    </row>
-    <row r="27" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F26" s="8"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>25</v>
       </c>
       <c r="B27" s="4">
-        <v>44637</v>
+        <v>44272</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E27" s="8"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="5"/>
-    </row>
-    <row r="28" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F27" s="8"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="5"/>
+    </row>
+    <row r="28" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>26</v>
       </c>
       <c r="B28" s="4">
-        <v>44644</v>
+        <v>44279</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E28" s="8"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="5"/>
-    </row>
-    <row r="29" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F28" s="8"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="5"/>
+    </row>
+    <row r="29" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>27</v>
       </c>
       <c r="B29" s="4">
-        <v>44651</v>
+        <v>44286</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E29" s="8"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="5"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F29" s="8"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="5"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>28</v>
       </c>
       <c r="B30" s="4">
-        <v>44658</v>
+        <v>44293</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E30" s="7"/>
-      <c r="G30" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H30" s="3"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F30" s="7"/>
+      <c r="H30" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30" s="3"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>29</v>
       </c>
       <c r="B31" s="4">
-        <v>44665</v>
+        <v>44300</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E31" s="7"/>
-      <c r="G31" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H31" s="3"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F31" s="7"/>
+      <c r="H31" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>30</v>
       </c>
       <c r="B32" s="4">
-        <v>44672</v>
+        <v>44307</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E32" s="7"/>
-      <c r="G32" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H32" s="3"/>
-    </row>
-    <row r="33" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F32" s="7"/>
+      <c r="H32" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I32" s="3"/>
+    </row>
+    <row r="33" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>31</v>
       </c>
       <c r="B33" s="4">
-        <v>44679</v>
+        <v>44314</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E33" s="8"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="5"/>
-    </row>
-    <row r="34" spans="1:8" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F33" s="8"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="5"/>
+    </row>
+    <row r="34" spans="1:9" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>32</v>
       </c>
       <c r="B34" s="4">
-        <v>44686</v>
+        <v>44321</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E34" s="8"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="5"/>
-    </row>
-    <row r="35" spans="1:8" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F34" s="8"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="1:9" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>33</v>
       </c>
       <c r="B35" s="4">
-        <v>44693</v>
+        <v>44328</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E35" s="8"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="5"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F35" s="8"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="5"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>34</v>
       </c>
       <c r="B36" s="4">
-        <v>44700</v>
+        <v>44335</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E36" s="7"/>
-      <c r="G36" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H36" s="3"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F36" s="7"/>
+      <c r="H36" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I36" s="3"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="6">
         <v>35</v>
       </c>
       <c r="B37" s="4">
-        <v>44707</v>
+        <v>44342</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E37" s="7"/>
-      <c r="G37" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H37" s="3"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F37" s="7"/>
+      <c r="H37" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I37" s="3"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>36</v>
       </c>
       <c r="B38" s="4">
-        <v>44714</v>
+        <v>44349</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E38" s="7"/>
-      <c r="G38" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H38" s="3"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F38" s="7"/>
+      <c r="H38" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I38" s="3"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B39" s="1"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B40" s="1"/>
       <c r="C40" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D40">
         <f>SUM(D2:D38)</f>
         <v>0</v>
       </c>
-      <c r="H40" cm="1">
-        <f t="array" aca="1" ref="H40" ca="1">A1:H40</f>
+      <c r="I40" cm="1">
+        <f t="array" aca="1" ref="I40" ca="1">A1:I40</f>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B41" s="1"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B42" s="1"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A48" s="13"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="13"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A49" s="14"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="14"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A50" s="15"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="15"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A51" s="15"/>
+      <c r="B51" s="16"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="17"/>
+      <c r="I51" s="15"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A52" s="15"/>
+      <c r="B52" s="16"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="15"/>
+      <c r="G52" s="15"/>
+      <c r="H52" s="17"/>
+      <c r="I52" s="15"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A53" s="15"/>
+      <c r="B53" s="16"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="15"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A54" s="15"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="15"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A55" s="15"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A56" s="15"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="15"/>
+      <c r="G56" s="15"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="15"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A57" s="15"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="15"/>
+      <c r="I57" s="15"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A58" s="15"/>
+      <c r="B58" s="16"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="17"/>
+      <c r="I58" s="15"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A59" s="15"/>
+      <c r="B59" s="16"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="17"/>
+      <c r="I59" s="17"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A60" s="15"/>
+      <c r="B60" s="16"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="15"/>
+      <c r="F60" s="15"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="17"/>
+      <c r="I60" s="15"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A61" s="15"/>
+      <c r="B61" s="16"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="15"/>
+      <c r="F61" s="15"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="17"/>
+      <c r="I61" s="15"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A62" s="15"/>
+      <c r="B62" s="16"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="15"/>
+      <c r="I62" s="15"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A63" s="15"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="15"/>
+      <c r="I63" s="15"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A64" s="15"/>
+      <c r="B64" s="16"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="15"/>
+      <c r="H64" s="15"/>
+      <c r="I64" s="15"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A65" s="15"/>
+      <c r="B65" s="16"/>
+      <c r="C65" s="15"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="15"/>
+      <c r="F65" s="15"/>
+      <c r="G65" s="15"/>
+      <c r="H65" s="15"/>
+      <c r="I65" s="15"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A66" s="15"/>
+      <c r="B66" s="16"/>
+      <c r="C66" s="15"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="15"/>
+      <c r="F66" s="15"/>
+      <c r="G66" s="15"/>
+      <c r="H66" s="15"/>
+      <c r="I66" s="15"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A67" s="15"/>
+      <c r="B67" s="16"/>
+      <c r="C67" s="15"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="15"/>
+      <c r="G67" s="15"/>
+      <c r="H67" s="15"/>
+      <c r="I67" s="15"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A68" s="15"/>
+      <c r="B68" s="16"/>
+      <c r="C68" s="15"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="15"/>
+      <c r="F68" s="15"/>
+      <c r="G68" s="15"/>
+      <c r="H68" s="15"/>
+      <c r="I68" s="15"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A69" s="15"/>
+      <c r="B69" s="16"/>
+      <c r="C69" s="15"/>
+      <c r="D69" s="15"/>
+      <c r="E69" s="15"/>
+      <c r="F69" s="15"/>
+      <c r="G69" s="15"/>
+      <c r="H69" s="15"/>
+      <c r="I69" s="15"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A70" s="15"/>
+      <c r="B70" s="16"/>
+      <c r="C70" s="15"/>
+      <c r="D70" s="15"/>
+      <c r="E70" s="15"/>
+      <c r="F70" s="15"/>
+      <c r="G70" s="15"/>
+      <c r="H70" s="15"/>
+      <c r="I70" s="15"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A71" s="15"/>
+      <c r="B71" s="16"/>
+      <c r="C71" s="15"/>
+      <c r="D71" s="15"/>
+      <c r="E71" s="15"/>
+      <c r="F71" s="15"/>
+      <c r="G71" s="15"/>
+      <c r="H71" s="15"/>
+      <c r="I71" s="15"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A72" s="15"/>
+      <c r="B72" s="16"/>
+      <c r="C72" s="15"/>
+      <c r="D72" s="15"/>
+      <c r="E72" s="15"/>
+      <c r="F72" s="15"/>
+      <c r="G72" s="15"/>
+      <c r="H72" s="15"/>
+      <c r="I72" s="15"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A73" s="15"/>
+      <c r="B73" s="16"/>
+      <c r="C73" s="15"/>
+      <c r="D73" s="15"/>
+      <c r="E73" s="15"/>
+      <c r="F73" s="15"/>
+      <c r="G73" s="15"/>
+      <c r="H73" s="15"/>
+      <c r="I73" s="15"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A74" s="15"/>
+      <c r="B74" s="16"/>
+      <c r="C74" s="15"/>
+      <c r="D74" s="15"/>
+      <c r="E74" s="15"/>
+      <c r="F74" s="15"/>
+      <c r="G74" s="15"/>
+      <c r="H74" s="15"/>
+      <c r="I74" s="15"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A75" s="15"/>
+      <c r="B75" s="16"/>
+      <c r="C75" s="15"/>
+      <c r="D75" s="15"/>
+      <c r="E75" s="15"/>
+      <c r="F75" s="15"/>
+      <c r="G75" s="15"/>
+      <c r="H75" s="15"/>
+      <c r="I75" s="15"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A76" s="15"/>
+      <c r="B76" s="16"/>
+      <c r="C76" s="15"/>
+      <c r="D76" s="15"/>
+      <c r="E76" s="15"/>
+      <c r="F76" s="15"/>
+      <c r="G76" s="15"/>
+      <c r="H76" s="15"/>
+      <c r="I76" s="15"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A77" s="15"/>
+      <c r="B77" s="16"/>
+      <c r="C77" s="15"/>
+      <c r="D77" s="15"/>
+      <c r="E77" s="15"/>
+      <c r="F77" s="15"/>
+      <c r="G77" s="15"/>
+      <c r="H77" s="15"/>
+      <c r="I77" s="15"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A78" s="15"/>
+      <c r="B78" s="16"/>
+      <c r="C78" s="15"/>
+      <c r="D78" s="15"/>
+      <c r="E78" s="15"/>
+      <c r="F78" s="15"/>
+      <c r="G78" s="15"/>
+      <c r="H78" s="15"/>
+      <c r="I78" s="15"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A79" s="15"/>
+      <c r="B79" s="16"/>
+      <c r="C79" s="15"/>
+      <c r="D79" s="15"/>
+      <c r="E79" s="15"/>
+      <c r="F79" s="15"/>
+      <c r="G79" s="15"/>
+      <c r="H79" s="15"/>
+      <c r="I79" s="15"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A80" s="15"/>
+      <c r="B80" s="16"/>
+      <c r="C80" s="15"/>
+      <c r="D80" s="15"/>
+      <c r="E80" s="15"/>
+      <c r="F80" s="15"/>
+      <c r="G80" s="15"/>
+      <c r="H80" s="15"/>
+      <c r="I80" s="15"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A81" s="15"/>
+      <c r="B81" s="16"/>
+      <c r="C81" s="15"/>
+      <c r="D81" s="15"/>
+      <c r="E81" s="15"/>
+      <c r="F81" s="15"/>
+      <c r="G81" s="15"/>
+      <c r="H81" s="15"/>
+      <c r="I81" s="15"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A82" s="15"/>
+      <c r="B82" s="16"/>
+      <c r="C82" s="15"/>
+      <c r="D82" s="15"/>
+      <c r="E82" s="15"/>
+      <c r="F82" s="15"/>
+      <c r="G82" s="15"/>
+      <c r="H82" s="15"/>
+      <c r="I82" s="15"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A83" s="15"/>
+      <c r="B83" s="16"/>
+      <c r="C83" s="15"/>
+      <c r="D83" s="15"/>
+      <c r="E83" s="15"/>
+      <c r="F83" s="15"/>
+      <c r="G83" s="15"/>
+      <c r="H83" s="15"/>
+      <c r="I83" s="15"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A84" s="15"/>
+      <c r="B84" s="16"/>
+      <c r="C84" s="15"/>
+      <c r="D84" s="15"/>
+      <c r="E84" s="15"/>
+      <c r="F84" s="15"/>
+      <c r="G84" s="15"/>
+      <c r="H84" s="15"/>
+      <c r="I84" s="15"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A85" s="15"/>
+      <c r="B85" s="16"/>
+      <c r="C85" s="15"/>
+      <c r="D85" s="15"/>
+      <c r="E85" s="15"/>
+      <c r="F85" s="15"/>
+      <c r="G85" s="15"/>
+      <c r="H85" s="15"/>
+      <c r="I85" s="15"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A86" s="15"/>
+      <c r="B86" s="16"/>
+      <c r="C86" s="15"/>
+      <c r="D86" s="15"/>
+      <c r="E86" s="15"/>
+      <c r="F86" s="15"/>
+      <c r="G86" s="15"/>
+      <c r="H86" s="15"/>
+      <c r="I86" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>